<commit_message>
fixed typo in office hour schedule
</commit_message>
<xml_diff>
--- a/OfficeHoursSchedule.xlsx
+++ b/OfficeHoursSchedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\metin\Documents\nufintech\nu-chi-fin-pt-04-2020-u-c\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C40A431-9FB3-4607-AACD-10222B35802A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B7A8842-42DA-4B3C-9E38-DA7F48874BA1}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="OfficeHoursSchedule" sheetId="3" r:id="rId1"/>
@@ -51,9 +51,6 @@
     <t>Saturday</t>
   </si>
   <si>
-    <t>Week 1</t>
-  </si>
-  <si>
     <t>Day</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t xml:space="preserve">Kumari Amrita </t>
+  </si>
+  <si>
+    <t>Week 3</t>
   </si>
 </sst>
 </file>
@@ -497,7 +497,7 @@
   <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -507,13 +507,13 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" t="s">
         <v>7</v>
-      </c>
-      <c r="C1" t="s">
-        <v>8</v>
       </c>
       <c r="D1" t="s">
         <v>0</v>
@@ -521,7 +521,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -535,7 +535,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B3" t="s">
         <v>1</v>
@@ -549,7 +549,7 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -563,7 +563,7 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B5" t="s">
         <v>3</v>
@@ -577,7 +577,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B6" t="s">
         <v>1</v>
@@ -591,7 +591,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -605,7 +605,7 @@
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
         <v>3</v>
@@ -619,7 +619,7 @@
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" t="s">
         <v>1</v>
@@ -633,7 +633,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -647,7 +647,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" t="s">
         <v>3</v>
@@ -661,7 +661,7 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>1</v>
@@ -675,7 +675,7 @@
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -689,7 +689,7 @@
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" t="s">
         <v>3</v>
@@ -703,7 +703,7 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
         <v>1</v>
@@ -717,7 +717,7 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B16" t="s">
         <v>2</v>
@@ -731,7 +731,7 @@
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" t="s">
         <v>3</v>
@@ -745,7 +745,7 @@
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B18" t="s">
         <v>1</v>
@@ -759,7 +759,7 @@
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>

</xml_diff>